<commit_message>
Add cantrals by cantons
</commit_message>
<xml_diff>
--- a/Project/Data/Water/Cantons/AG/AG 2006.xlsx
+++ b/Project/Data/Water/Cantons/AG/AG 2006.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>(m3/s)</t>
   </si>
@@ -117,15 +117,6 @@
   </si>
   <si>
     <t>Beznau-Wehrkraftwerk</t>
-  </si>
-  <si>
-    <t>1'315.66</t>
-  </si>
-  <si>
-    <t>1'653.91</t>
-  </si>
-  <si>
-    <t>2'969.56</t>
   </si>
   <si>
     <t>idx</t>
@@ -588,44 +579,44 @@
   <dimension ref="A1:K84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:K1"/>
+      <selection activeCell="G33" sqref="G33:K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
         <v>35</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>36</v>
-      </c>
-      <c r="C1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" t="s">
-        <v>39</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -1672,23 +1663,6 @@
       </c>
       <c r="K32" s="3">
         <v>35.5</v>
-      </c>
-    </row>
-    <row r="33" spans="7:11">
-      <c r="G33" s="3">
-        <v>497.43</v>
-      </c>
-      <c r="H33" s="3">
-        <v>475.52</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J33" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K33" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="84" spans="1:2">

</xml_diff>